<commit_message>
made config similar for excel and googlesheets
</commit_message>
<xml_diff>
--- a/nodejs/excel/test/test_data.xlsx
+++ b/nodejs/excel/test/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BA9ED1-FE22-42C4-91BB-B23E6470119C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B50DE9-93D6-4B63-B255-25D65656E3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>S.No.</t>
   </si>
@@ -150,6 +150,24 @@
   </si>
   <si>
     <t>S_1_1</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>t0</t>
+  </si>
+  <si>
+    <t>o0</t>
+  </si>
+  <si>
+    <t>c0</t>
+  </si>
+  <si>
+    <t>in0</t>
+  </si>
+  <si>
+    <t>r0</t>
   </si>
 </sst>
 </file>
@@ -220,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,12 +255,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -263,9 +275,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -555,8 +564,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,37 +608,37 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,7 +686,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -693,239 +702,251 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="A3" s="7">
+        <v>0</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -936,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187DE655-AA37-44E9-B1C5-DA9AD2DB6309}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
improve excel file to csv converter
</commit_message>
<xml_diff>
--- a/nodejs/excel/test/test_data.xlsx
+++ b/nodejs/excel/test/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B50DE9-93D6-4B63-B255-25D65656E3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2CB20E-5319-4D6B-9F59-88EA6414F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
     <sheet name="test-2" sheetId="2" r:id="rId2"/>
     <sheet name="test-3" sheetId="7" r:id="rId3"/>
+    <sheet name="test-4" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>S.No.</t>
   </si>
@@ -168,6 +169,66 @@
   </si>
   <si>
     <t>r0</t>
+  </si>
+  <si>
+    <t>Ok-one</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Six</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>Fourteen</t>
+  </si>
+  <si>
+    <t>Fiftin</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>A
+B
+C
+D
+E
+F
+G</t>
   </si>
 </sst>
 </file>
@@ -238,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -278,6 +339,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,8 +631,8 @@
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,4 +1126,147 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326B7AE-969A-4E5C-9DC5-55FF350E7668}">
+  <dimension ref="A2:V15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="G7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="M10" t="s">
+        <v>50</v>
+      </c>
+      <c r="N10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="P11" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="R12" t="s">
+        <v>59</v>
+      </c>
+      <c r="S12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="T13" t="s">
+        <v>61</v>
+      </c>
+      <c r="U13" t="s">
+        <v>62</v>
+      </c>
+      <c r="V13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improved excel file reading by removing limitation of comma and new line for the first line
</commit_message>
<xml_diff>
--- a/nodejs/excel/test/test_data.xlsx
+++ b/nodejs/excel/test/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2CB20E-5319-4D6B-9F59-88EA6414F2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C03F70-BEAA-4863-84BE-3C8B8C71EE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>S.No.</t>
   </si>
@@ -72,9 +72,6 @@
     <t>on_route</t>
   </si>
   <si>
-    <t>conflicting</t>
-  </si>
-  <si>
     <t>in_isolation</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>t0</t>
   </si>
   <si>
-    <t>o0</t>
-  </si>
-  <si>
     <t>c0</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
   </si>
   <si>
     <t>r0</t>
-  </si>
-  <si>
-    <t>Ok-one</t>
   </si>
   <si>
     <t>One</t>
@@ -230,12 +221,40 @@
 F
 G</t>
   </si>
+  <si>
+    <t>o0,o2</t>
+  </si>
+  <si>
+    <t>conflicting, signal</t>
+  </si>
+  <si>
+    <t>Six
+B
+C
+D
+E</t>
+  </si>
+  <si>
+    <t>Seven
+C
+D
+E</t>
+  </si>
+  <si>
+    <t>one
+C
+D
+E</t>
+  </si>
+  <si>
+    <t>Ok,one</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +269,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -299,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -338,13 +364,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,7 +661,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,37 +704,37 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -751,9 +780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5FB583-A461-4C0D-8684-41D0A89D5DCC}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,13 +811,13 @@
         <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
@@ -796,22 +825,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -819,29 +848,29 @@
         <v>0</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="D4" s="15"/>
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
@@ -1037,37 +1066,37 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" t="s">
-        <v>35</v>
-      </c>
       <c r="R1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -1084,43 +1113,43 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
       <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
         <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>37</v>
-      </c>
-      <c r="R2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1133,81 +1162,81 @@
   <dimension ref="A2:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
-        <v>47</v>
+    <row r="2" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="S2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="G7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
@@ -1217,53 +1246,53 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="K9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="M10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" t="s">
         <v>50</v>
-      </c>
-      <c r="N10" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="P11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="R12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="S12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="T13" t="s">
+        <v>58</v>
+      </c>
+      <c r="U13" t="s">
+        <v>59</v>
+      </c>
+      <c r="V13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="U13" t="s">
-        <v>62</v>
-      </c>
-      <c r="V13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved dbview and dbview_summary rendering by making it faster
</commit_message>
<xml_diff>
--- a/nodejs/excel/test/test_data.xlsx
+++ b/nodejs/excel/test/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C03F70-BEAA-4863-84BE-3C8B8C71EE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEEE5A6-8EE6-4333-B1D8-F161F6C44AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
@@ -271,7 +271,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -325,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -369,8 +368,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -704,37 +709,37 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -780,9 +785,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5FB583-A461-4C0D-8684-41D0A89D5DCC}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -867,10 +872,18 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="7">
+        <v>12</v>
+      </c>
+      <c r="B4" s="15">
+        <v>45152</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0.96736111111111101</v>
+      </c>
+      <c r="D4" s="16">
+        <v>45152.979166666664</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
@@ -1161,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326B7AE-969A-4E5C-9DC5-55FF350E7668}">
   <dimension ref="A2:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
java roles mapping app improved
</commit_message>
<xml_diff>
--- a/nodejs/excel/test/test_data.xlsx
+++ b/nodejs/excel/test/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\project\nodejs\excel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CEEE5A6-8EE6-4333-B1D8-F161F6C44AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F33B40B-203C-41D6-9DEE-3EC2177534D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +293,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -351,13 +363,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -365,12 +371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -379,6 +379,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,17 +695,17 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.36328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7265625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="5.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -708,38 +734,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
@@ -750,17 +776,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -785,28 +811,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5FB583-A461-4C0D-8684-41D0A89D5DCC}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.6328125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.90625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.81640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8" style="23" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -815,7 +841,7 @@
       <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -825,11 +851,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="59" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+    <row r="2" spans="1:7" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="21" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -838,7 +864,7 @@
       <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="21" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -848,11 +874,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="20">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -861,7 +887,7 @@
       <c r="D3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="21" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -871,191 +897,191 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="20">
         <v>12</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="22">
         <v>45152</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="13">
         <v>0.96736111111111101</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <v>45152.979166666664</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-    </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-    </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1066,18 +1092,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{187DE655-AA37-44E9-B1C5-DA9AD2DB6309}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="13.26953125" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" customWidth="1"/>
-    <col min="15" max="15" width="12.36328125" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1112,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1175,22 +1201,27 @@
   <dimension ref="A2:V15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="15"/>
+    <col min="4" max="4" width="8.88671875" style="18"/>
+    <col min="5" max="5" width="8.88671875" style="15"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:22" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
         <v>67</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>64</v>
       </c>
       <c r="G2" t="s">
@@ -1199,52 +1230,52 @@
       <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="11" t="s">
         <v>66</v>
       </c>
       <c r="S2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>50</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="F5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G7" t="s">
         <v>52</v>
       </c>
@@ -1252,12 +1283,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="J8">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="K9" t="s">
         <v>54</v>
       </c>
@@ -1265,7 +1296,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M10" t="s">
         <v>47</v>
       </c>
@@ -1276,7 +1307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="P11" t="s">
         <v>46</v>
       </c>
@@ -1284,7 +1315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="R12" t="s">
         <v>56</v>
       </c>
@@ -1292,7 +1323,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="T13" t="s">
         <v>58</v>
       </c>
@@ -1303,8 +1334,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:22" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>